<commit_message>
updated zip file for package
</commit_message>
<xml_diff>
--- a/output/results-processing.xlsx
+++ b/output/results-processing.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="2020" windowWidth="14400" windowHeight="16460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20020" yWindow="7700" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rsquarechange-se.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="semirtable.csv" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>estimator</t>
   </si>
@@ -83,14 +84,138 @@
   </si>
   <si>
     <t>sort order</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>facet</t>
+  </si>
+  <si>
+    <t>r_zero_order</t>
+  </si>
+  <si>
+    <t>sr_focal_factor</t>
+  </si>
+  <si>
+    <t>sr_all_factors</t>
+  </si>
+  <si>
+    <t>sr_other_facets</t>
+  </si>
+  <si>
+    <t>ipip_neuroticism</t>
+  </si>
+  <si>
+    <t>ipip_n_anxiety</t>
+  </si>
+  <si>
+    <t>ipip_n_anger</t>
+  </si>
+  <si>
+    <t>ipip_n_depression</t>
+  </si>
+  <si>
+    <t>ipip_n_self_consciousness</t>
+  </si>
+  <si>
+    <t>ipip_n_immoderation</t>
+  </si>
+  <si>
+    <t>ipip_n_vulnerability</t>
+  </si>
+  <si>
+    <t>ipip_extraversion</t>
+  </si>
+  <si>
+    <t>ipip_e_friendliness</t>
+  </si>
+  <si>
+    <t>ipip_e_gregariousness</t>
+  </si>
+  <si>
+    <t>ipip_e_assertiveness</t>
+  </si>
+  <si>
+    <t>ipip_e_activity_level</t>
+  </si>
+  <si>
+    <t>ipip_e_excitement_seeking</t>
+  </si>
+  <si>
+    <t>ipip_e_cheerfulness</t>
+  </si>
+  <si>
+    <t>ipip_openness</t>
+  </si>
+  <si>
+    <t>ipip_o_imagination</t>
+  </si>
+  <si>
+    <t>ipip_o_artistic_interests</t>
+  </si>
+  <si>
+    <t>ipip_o_emotionality</t>
+  </si>
+  <si>
+    <t>ipip_o_adventurousness</t>
+  </si>
+  <si>
+    <t>ipip_o_intellect</t>
+  </si>
+  <si>
+    <t>ipip_o_liberalism</t>
+  </si>
+  <si>
+    <t>ipip_agreeableness</t>
+  </si>
+  <si>
+    <t>ipip_a_trust</t>
+  </si>
+  <si>
+    <t>ipip_a_morality</t>
+  </si>
+  <si>
+    <t>ipip_a_altruism</t>
+  </si>
+  <si>
+    <t>ipip_a_cooperation</t>
+  </si>
+  <si>
+    <t>ipip_a_modesty</t>
+  </si>
+  <si>
+    <t>ipip_a_sympathy</t>
+  </si>
+  <si>
+    <t>ipip_conscientiousness</t>
+  </si>
+  <si>
+    <t>ipip_c_self_efficacy</t>
+  </si>
+  <si>
+    <t>ipip_c_orderliness</t>
+  </si>
+  <si>
+    <t>ipip_c_dutifulness</t>
+  </si>
+  <si>
+    <t>ipip_c_achievement_striving</t>
+  </si>
+  <si>
+    <t>ipip_c_self_discipline</t>
+  </si>
+  <si>
+    <t>ipip_c_cautiousness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode=".000"/>
+    <numFmt numFmtId="165" formatCode=".00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -203,9 +328,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1310,9 +1436,739 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-0.47231087951144002</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.02633640004244E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.79644417687428E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.4231979347564201E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.31294682617372799</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.155805493875708</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.0199250668114898E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.2765875781723999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-0.67338808285584795</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-0.35288091366391899</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-0.27984235223655002</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-0.224598852048078</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-0.46153441835903602</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-5.0695558641409302E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.140815325737112</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.6349280908217301E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-0.155475062136608</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.17141483822512499</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.8832568772965498E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.6722100999526999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-0.48895018028112702</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-8.3161858835581904E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.81001947511999E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-3.3622808374773702E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.44294019032521598</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.5362172892749302E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-3.4648916527586497E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-5.4126944426100602E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.33876086693205598</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-0.13899306600813499</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-5.19401398311145E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.4018466603899698E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.38645737438743699</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-1.05347957920811E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-8.1083865137258002E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-1.9502344847701199E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.33258336170462299</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8.8557751429711104E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-2.4646405032582901E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-2.2314413391851501E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.20906275655092299</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-0.17203718676312299</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-3.3146803603282898E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.6405699025809E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.56861759851090798</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.27034950715297301</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.25649400717134702</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.17523470193044999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.9138167204969803E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-4.7958709814730001E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6.8780636746765295E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-1.4150138844830299E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6.3901569899686997E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-2.4129027037998001E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-7.8750781576195292E-3</v>
+      </c>
+      <c r="G15" s="2">
+        <v>6.5326002947584203E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.9213867288123203E-3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-0.10103883069908499</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.5940816865094601E-2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-1.36400445079847E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.273607328121171</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.246415330866704</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-8.5339190711332096E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-1.5745416065244499E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.18074383998621499</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.130585344959434</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-5.5961408877875797E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-3.4323936892154301E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-9.8252211899142003E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-0.20196584983913099</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-2.9211518904818601E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-2.55175297003262E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.353449780315851</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.356734449953722</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5.0405487394542897E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-1.50220591204518E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4.6960611221392702E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-6.5481290668721506E-2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-2.3650575595331302E-2</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-4.9623385586765802E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.26217988042783402</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.27476646712852498</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-7.2332012558483398E-3</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-1.13744795092415E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2">
+        <v>7.2373811663379195E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-2.3716516819197599E-2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>3.1635614940126101E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3.07047818128257E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="2">
+        <v>-0.31647090312173298</v>
+      </c>
+      <c r="E24" s="2">
+        <v>-0.44806912123995102</v>
+      </c>
+      <c r="F24" s="2">
+        <v>-0.10550231237369299</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-2.2268141778805602E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.5549732169581796E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>7.5256763077544305E-4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>7.1452587245413202E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>4.4537764878734599E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.48607210955774799</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.33789120949310802</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.6356532866368199E-2</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3.7503424755794601E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2">
+        <v>7.0398309192945902E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-0.28029352760894599</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-9.3207981111740598E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-7.57291671027671E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.14069103799865201</v>
+      </c>
+      <c r="E28" s="2">
+        <v>-0.15736174755749799</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-8.6644632531823099E-2</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-5.2424329622447502E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.42030170092904601</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.23436880469372001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.132626515806716</v>
+      </c>
+      <c r="G29" s="2">
+        <v>9.9056179418145998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.40552176985034399</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.20596628348683499</v>
+      </c>
+      <c r="F30" s="2">
+        <v>4.6173315448698203E-2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4.0667333952317003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6.1515518457071899E-2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>-0.23872937132701399</v>
+      </c>
+      <c r="F31" s="2">
+        <v>-1.2340763520237099E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4.0799167311740103E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>